<commit_message>
imporved consistancy across repo, updated openfast model
</commit_message>
<xml_diff>
--- a/Documentation/RNA_modeling_properties.xlsx
+++ b/Documentation/RNA_modeling_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/banderso2/Documents/Office/15MW/Drivetrain Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\IEA-15-240-RWT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7EA351-88D5-9B46-8323-6693A8C2A650}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F756B8-E5EB-441F-9483-9ED1031C3FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="580" windowWidth="38400" windowHeight="19600" xr2:uid="{F4F21123-4A90-4967-8B8F-5B3BBB50E9DF}"/>
+    <workbookView xWindow="32160" yWindow="3360" windowWidth="21600" windowHeight="11265" xr2:uid="{F4F21123-4A90-4967-8B8F-5B3BBB50E9DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -296,8 +294,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -406,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,8 +420,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -436,6 +433,12 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +467,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>152737</xdr:colOff>
+      <xdr:colOff>101937</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>183232</xdr:rowOff>
     </xdr:to>
@@ -799,23 +802,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4482DD-C7A9-4488-B769-C91931618407}">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="80.1640625" customWidth="1"/>
-    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="80.1796875" customWidth="1"/>
+    <col min="18" max="18" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16">
+    <row r="1" spans="1:15" ht="15.5">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -832,7 +836,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:15" ht="16">
+    <row r="2" spans="1:15" ht="15.5">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -853,7 +857,7 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="16">
+    <row r="3" spans="1:15" ht="15.5">
       <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
@@ -870,7 +874,7 @@
       <c r="G3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="15">
         <f>4.34781123</f>
         <v>4.3478112299999996</v>
       </c>
@@ -886,7 +890,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="16">
+    <row r="4" spans="1:15" ht="15.5">
       <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
@@ -903,7 +907,7 @@
       <c r="G4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <v>11.35271202</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -918,7 +922,7 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="16">
+    <row r="5" spans="1:15" ht="15.5">
       <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
@@ -934,7 +938,7 @@
       <c r="G5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>0.38</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -947,7 +951,7 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="16">
+    <row r="6" spans="1:15" ht="15.5">
       <c r="A6" s="8" t="s">
         <v>42</v>
       </c>
@@ -961,7 +965,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="16"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -970,7 +974,7 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="16">
+    <row r="7" spans="1:15" ht="15.5">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
@@ -986,7 +990,7 @@
       <c r="G7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -995,7 +999,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="16">
+    <row r="8" spans="1:15" ht="15.5">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -1011,7 +1015,7 @@
       <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -1020,7 +1024,7 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="16">
+    <row r="9" spans="1:15" ht="15.5">
       <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
@@ -1036,7 +1040,7 @@
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="28">
         <f>B11</f>
         <v>190000</v>
       </c>
@@ -1050,7 +1054,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="16">
+    <row r="10" spans="1:15" ht="15.5">
       <c r="A10" s="8" t="s">
         <v>39</v>
       </c>
@@ -1066,7 +1070,7 @@
       <c r="G10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="16">
         <v>1373471.226</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -1079,7 +1083,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="16">
+    <row r="11" spans="1:15" ht="15.5">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1095,7 +1099,7 @@
       <c r="G11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="25">
         <f xml:space="preserve"> 4716092+ 3292558</f>
         <v>8008650</v>
       </c>
@@ -1109,12 +1113,12 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="16">
+    <row r="12" spans="1:15" ht="15.5">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="8">
-        <v>204000</v>
+        <v>191335.49077422</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>44</v>
@@ -1140,7 +1144,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="16">
+    <row r="13" spans="1:15" ht="15.5">
       <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
@@ -1156,7 +1160,7 @@
       <c r="G13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="25">
         <v>0</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1171,7 +1175,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="16">
+    <row r="14" spans="1:15" ht="15.5">
       <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
@@ -1203,24 +1207,24 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" ht="16">
+    <row r="15" spans="1:15" ht="15.5">
       <c r="A15" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="9">
         <f>SUM(B3:B14)</f>
-        <v>1001275.0249999999</v>
+        <v>988610.51577421988</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="25">
         <f>507275.04</f>
         <v>507275.04</v>
       </c>
@@ -1236,7 +1240,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" ht="16">
+    <row r="16" spans="1:15" ht="15.5">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1246,7 +1250,7 @@
       <c r="G16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="26">
         <f xml:space="preserve"> 19617857.267</f>
         <v>19617857.267000001</v>
       </c>
@@ -1262,7 +1266,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" ht="16">
+    <row r="17" spans="1:15" ht="15.5">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1272,7 +1276,7 @@
       <c r="G17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="27">
         <f>B9</f>
         <v>100000</v>
       </c>
@@ -1286,7 +1290,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="16">
+    <row r="18" spans="1:15" ht="15.5">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1296,7 +1300,7 @@
       <c r="G18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1305,7 +1309,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="16">
+    <row r="19" spans="1:15" ht="15.5">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1315,7 +1319,7 @@
       <c r="G19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="23">
         <v>6.8529999999999998</v>
       </c>
       <c r="I19" s="4" t="s">
@@ -1330,7 +1334,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:15" ht="16">
+    <row r="20" spans="1:15" ht="15.5">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1340,7 +1344,7 @@
       <c r="G20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="24">
         <v>0</v>
       </c>
       <c r="I20" s="7" t="s">
@@ -1353,7 +1357,7 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="16">
+    <row r="21" spans="1:15" ht="15.5">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1363,7 +1367,7 @@
       <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="23">
         <v>4.351</v>
       </c>
       <c r="I21" s="7" t="s">
@@ -1376,7 +1380,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="16">
+    <row r="22" spans="1:15" ht="15.5">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1386,7 +1390,7 @@
       <c r="G22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="20">
         <f>26505193.242+374349414</f>
         <v>400854607.24199998</v>
       </c>
@@ -1400,7 +1404,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" ht="16">
+    <row r="23" spans="1:15" ht="15.5">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1410,7 +1414,7 @@
       <c r="G23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="20">
         <f xml:space="preserve"> 60244378.133+178808930</f>
         <v>239053308.13300002</v>
       </c>
@@ -1424,7 +1428,7 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" ht="16">
+    <row r="24" spans="1:15" ht="15.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1434,7 +1438,7 @@
       <c r="G24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="20">
         <f>44447135.39+140448150</f>
         <v>184895285.38999999</v>
       </c>
@@ -1448,7 +1452,7 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" ht="16">
+    <row r="25" spans="1:15" ht="15.5">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1458,7 +1462,7 @@
       <c r="G25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="22">
         <v>20.763999999999999</v>
       </c>
       <c r="I25" s="7" t="s">
@@ -1473,7 +1477,7 @@
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="16">
+    <row r="26" spans="1:15" ht="15.5">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1483,7 +1487,7 @@
       <c r="G26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="22">
         <v>23356749.076000001</v>
       </c>
       <c r="I26" s="7" t="s">
@@ -1496,7 +1500,7 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" ht="16">
+    <row r="27" spans="1:15" ht="15.5">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1506,7 +1510,7 @@
       <c r="G27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="22">
         <v>23.878</v>
       </c>
       <c r="I27" s="7" t="s">
@@ -1521,7 +1525,7 @@
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" ht="16">
+    <row r="28" spans="1:15" ht="15.5">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1531,7 +1535,7 @@
       <c r="G28" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="20"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="4"/>
@@ -1540,7 +1544,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="16">
+    <row r="29" spans="1:15" ht="15.5">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1550,7 +1554,7 @@
       <c r="G29" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="20">
         <v>-5.9710000000000001</v>
       </c>
       <c r="I29" s="7" t="s">
@@ -1563,7 +1567,7 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" ht="16">
+    <row r="30" spans="1:15" ht="15.5">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1573,7 +1577,7 @@
       <c r="G30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="22">
+      <c r="H30" s="20">
         <f xml:space="preserve"> 10855262.338</f>
         <v>10855262.338</v>
       </c>
@@ -1589,7 +1593,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
     </row>
-    <row r="31" spans="1:15" ht="16">
+    <row r="31" spans="1:15" ht="15.5">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1599,7 +1603,7 @@
       <c r="G31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="21">
         <f xml:space="preserve">   8450907.645</f>
         <v>8450907.6449999996</v>
       </c>
@@ -1613,7 +1617,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" ht="16">
+    <row r="32" spans="1:15" ht="15.5">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1623,7 +1627,7 @@
       <c r="G32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H32" s="20">
+      <c r="H32" s="18">
         <f xml:space="preserve"> 8381527.92</f>
         <v>8381527.9199999999</v>
       </c>
@@ -1637,7 +1641,7 @@
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" ht="16">
+    <row r="33" spans="1:15" ht="15.5">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1645,7 +1649,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="19"/>
+      <c r="H33" s="17"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="4"/>
@@ -1654,7 +1658,7 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" ht="16">
+    <row r="34" spans="1:15" ht="15.5">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1664,7 +1668,7 @@
       <c r="G34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="19"/>
+      <c r="H34" s="17"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="4"/>
@@ -1673,7 +1677,7 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" ht="20">
+    <row r="35" spans="1:15" ht="19">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1683,7 +1687,7 @@
       <c r="G35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="20">
+      <c r="H35" s="18">
         <v>14088839309.283863</v>
       </c>
       <c r="I35" s="7" t="s">
@@ -1698,7 +1702,7 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" ht="16">
+    <row r="36" spans="1:15" ht="15.5">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1719,7 +1723,7 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" ht="16">
+    <row r="37" spans="1:15" ht="15.5">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1740,7 +1744,7 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" ht="16">
+    <row r="38" spans="1:15" ht="15.5">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1761,7 +1765,7 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" ht="16">
+    <row r="39" spans="1:15" ht="15.5">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1778,7 +1782,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" ht="16">
+    <row r="40" spans="1:15" ht="15.5">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1795,7 +1799,7 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" ht="16">
+    <row r="41" spans="1:15" ht="15.5">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1812,7 +1816,7 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" ht="16">
+    <row r="42" spans="1:15" ht="15.5">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1829,7 +1833,7 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" ht="16">
+    <row r="43" spans="1:15" ht="15.5">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1846,6 +1850,9 @@
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
     </row>
+    <row r="44" spans="1:15">
+      <c r="H44" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
corrected spar cap thickness for new blade design
</commit_message>
<xml_diff>
--- a/Documentation/RNA_modeling_properties.xlsx
+++ b/Documentation/RNA_modeling_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egaertne\IEA-15-240-RWT\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F756B8-E5EB-441F-9483-9ED1031C3FCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51748684-B5F3-4EC2-B2D7-D662740FA774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="3360" windowWidth="21600" windowHeight="11265" xr2:uid="{F4F21123-4A90-4967-8B8F-5B3BBB50E9DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4F21123-4A90-4967-8B8F-5B3BBB50E9DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,9 +467,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>101937</xdr:colOff>
+      <xdr:colOff>105112</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>183232</xdr:rowOff>
+      <xdr:rowOff>180057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -805,7 +805,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1118,7 +1118,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="8">
-        <v>191335.49077422</v>
+        <v>195760.42804389002</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>44</v>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B15" s="9">
         <f>SUM(B3:B14)</f>
-        <v>988610.51577421988</v>
+        <v>993035.45304388995</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>44</v>

</xml_diff>